<commit_message>
This should make Airbase a bit more robust
helps handle more inputs
</commit_message>
<xml_diff>
--- a/Documentation/Airbase Input Specification Document.xlsx
+++ b/Documentation/Airbase Input Specification Document.xlsx
@@ -126,13 +126,13 @@
     <t>Usually works but it depends on the input, wont work for INT</t>
   </si>
   <si>
-    <t>Generally accepted by MySQL/sometimes rejected by python</t>
-  </si>
-  <si>
     <t xml:space="preserve">NOTE:  INT values only accept number characters.  DECIMAL values accept numbers and periods, </t>
   </si>
   <si>
     <t>VARCHAR should accept every other character marked with "YES" in this document.  Input is case sensitive.</t>
+  </si>
+  <si>
+    <t>Generally not accepted by MySQL</t>
   </si>
 </sst>
 </file>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,11 +801,9 @@
         <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>30</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D15" s="7"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
@@ -817,9 +815,11 @@
         <v>20</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
@@ -862,7 +862,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -885,7 +885,7 @@
     </row>
     <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -895,7 +895,7 @@
     </row>
     <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>

</xml_diff>